<commit_message>
Adjustment CUM/KWh - PJC
</commit_message>
<xml_diff>
--- a/public/template/Meter Consumption.xlsx
+++ b/public/template/Meter Consumption.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\CAMR-Robinsons_Laravel-main\CAMR-Robinsons_Laravel-main\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baluy\Documents\GitHub\camr_pjc\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC48ACC-8DEC-4119-B8F7-0F218277BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5097A00F-FD2E-4AD6-8E95-CA765DB3C69A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1260" windowWidth="24240" windowHeight="13290" xr2:uid="{0125C2CC-56FE-4ABB-A7E4-A48064F91EF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,9 +60,6 @@
     <t>Multiplier</t>
   </si>
   <si>
-    <t>KWH</t>
-  </si>
-  <si>
     <t>Total KWh</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Building Description</t>
+  </si>
+  <si>
+    <t>KWh</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -532,7 +532,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -567,8 +567,8 @@
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
+      <c r="A9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B9">
         <f>SUM(H:H)</f>
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>